<commit_message>
novos ajustes de criacao da base final
</commit_message>
<xml_diff>
--- a/ceps.xlsx
+++ b/ceps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pythonProject\pythonProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eliel\OneDrive\Área de Trabalho\Busca_cep\Buscar_endereco\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E15179-75A8-497F-AEBA-C343B9AC997D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A20838-E9D1-4036-8F8C-10230B4EE09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8580" yWindow="825" windowWidth="18390" windowHeight="12615" xr2:uid="{94409B7B-65BC-4294-AA81-2D623351F001}"/>
+    <workbookView xWindow="8925" yWindow="600" windowWidth="18390" windowHeight="12615" xr2:uid="{94409B7B-65BC-4294-AA81-2D623351F001}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,18 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="10">
   <si>
     <t>CEP</t>
-  </si>
-  <si>
-    <t>Logradouro/Nome</t>
-  </si>
-  <si>
-    <t>Bairro/Distrito</t>
-  </si>
-  <si>
-    <t>Localidade/UF</t>
   </si>
   <si>
     <t>02739-000</t>
@@ -457,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B05D241-1B16-4DE5-B274-1AEFD16244E9}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:A50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,411 +459,255 @@
     <col min="1" max="16384" width="23.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>